<commit_message>
Not returning builtin table names for GetWorksheetNames() method
</commit_message>
<xml_diff>
--- a/src/LinqToExcel.Tests/ExcelFiles/Companies.xlsx
+++ b/src/LinqToExcel.Tests/ExcelFiles/Companies.xlsx
@@ -4,19 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="15315" windowHeight="13575" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="15315" windowHeight="13575" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ColumnMappings" sheetId="2" r:id="rId2"/>
     <sheet name="MoreCompanies" sheetId="3" r:id="rId3"/>
+    <sheet name="AutoFiltered" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AutoFiltered!$A$1:$D$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">AutoFiltered!$A$1:$B$6</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -824,7 +829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -896,4 +901,139 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6890</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>98</v>
+      </c>
+      <c r="D3" s="1">
+        <v>34554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>300</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6454</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>29839</v>
+      </c>
+      <c r="D5" s="1">
+        <v>19162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>22182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>39730</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>433</v>
+      </c>
+      <c r="D8" s="1">
+        <v>29456</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D8"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
can filter by null or non null values now in where clause
</commit_message>
<xml_diff>
--- a/src/LinqToExcel.Tests/ExcelFiles/Companies.xlsx
+++ b/src/LinqToExcel.Tests/ExcelFiles/Companies.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="15315" windowHeight="13575" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="15315" windowHeight="13575" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ColumnMappings" sheetId="2" r:id="rId2"/>
     <sheet name="MoreCompanies" sheetId="3" r:id="rId3"/>
     <sheet name="AutoFiltered" sheetId="4" r:id="rId4"/>
+    <sheet name="NullCells" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AutoFiltered!$A$1:$D$8</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -907,7 +908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1036,4 +1037,75 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6890</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1">
+        <v>34554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6454</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed issue in GetWorksheetNames() that was deleting aprostrophes when it was part of the name
</commit_message>
<xml_diff>
--- a/src/LinqToExcel.Tests/ExcelFiles/Companies.xlsx
+++ b/src/LinqToExcel.Tests/ExcelFiles/Companies.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="15315" windowHeight="13575" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="15315" windowHeight="13575" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="MoreCompanies" sheetId="3" r:id="rId3"/>
     <sheet name="AutoFiltered" sheetId="4" r:id="rId4"/>
     <sheet name="NullCells" sheetId="5" r:id="rId5"/>
+    <sheet name="Paul's Worksheet" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AutoFiltered!$A$1:$D$8</definedName>
@@ -135,8 +136,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -171,6 +172,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -249,6 +255,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -283,6 +290,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -458,21 +466,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -500,7 +508,7 @@
         <v>6890</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -514,7 +522,7 @@
         <v>34554</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -528,7 +536,7 @@
         <v>6454</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -542,7 +550,7 @@
         <v>19162</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -556,7 +564,7 @@
         <v>22182</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -570,7 +578,7 @@
         <v>39730</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -592,14 +600,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -611,7 +619,7 @@
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -637,7 +645,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -663,7 +671,7 @@
         <v>12268</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -689,7 +697,7 @@
         <v>36412</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -715,7 +723,7 @@
         <v>32350</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -741,7 +749,7 @@
         <v>28359</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -767,7 +775,7 @@
         <v>16710</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -793,7 +801,7 @@
         <v>38868</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -827,21 +835,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -869,7 +877,7 @@
         <v>6890</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -883,7 +891,7 @@
         <v>34554</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -905,21 +913,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -933,7 +941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -947,7 +955,7 @@
         <v>6890</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -961,7 +969,7 @@
         <v>34554</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -975,7 +983,7 @@
         <v>6454</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -989,7 +997,7 @@
         <v>19162</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1003,7 +1011,7 @@
         <v>22182</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1017,7 +1025,7 @@
         <v>39730</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1040,21 +1048,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1068,7 +1076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1082,7 +1090,7 @@
         <v>6890</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1093,7 +1101,7 @@
         <v>34554</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1108,4 +1116,16 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
not including named ranges in GetWorksheetNames() method
</commit_message>
<xml_diff>
--- a/src/LinqToExcel.Tests/ExcelFiles/Companies.xlsx
+++ b/src/LinqToExcel.Tests/ExcelFiles/Companies.xlsx
@@ -17,6 +17,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AutoFiltered!$A$1:$D$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">AutoFiltered!$A$1:$B$6</definedName>
+    <definedName name="Range1">'Paul''s Worksheet'!$A$1:$D$11</definedName>
+    <definedName name="Range2">'Paul''s Worksheet'!$A$1:$D$11</definedName>
+    <definedName name="Range3" localSheetId="5">'Paul''s Worksheet'!$E$5:$H$16</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1122,7 +1125,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:H16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
Added similar columns to excel column attribute, its help to read imprevisible files (force to get data).
</commit_message>
<xml_diff>
--- a/src/LinqToExcel.Tests/ExcelFiles/Companies.xlsx
+++ b/src/LinqToExcel.Tests/ExcelFiles/Companies.xlsx
@@ -1,35 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\OneDrive\Desktop\Projetos\GitHub\LinqToExcel\src\LinqToExcel.Tests\ExcelFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="15315" windowHeight="13575" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="15315" windowHeight="13575" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="ColumnMappings" sheetId="2" r:id="rId2"/>
-    <sheet name="MoreCompanies" sheetId="3" r:id="rId3"/>
-    <sheet name="AutoFiltered" sheetId="4" r:id="rId4"/>
-    <sheet name="NullCells" sheetId="5" r:id="rId5"/>
-    <sheet name="Paul's Worksheet" sheetId="6" r:id="rId6"/>
+    <sheet name="ColumnSimilarMappings" sheetId="7" r:id="rId2"/>
+    <sheet name="ColumnMappings" sheetId="2" r:id="rId3"/>
+    <sheet name="MoreCompanies" sheetId="3" r:id="rId4"/>
+    <sheet name="AutoFiltered" sheetId="4" r:id="rId5"/>
+    <sheet name="NullCells" sheetId="5" r:id="rId6"/>
+    <sheet name="Paul's Worksheet" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AutoFiltered!$A$1:$D$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">AutoFiltered!$A$1:$D$8</definedName>
     <definedName name="Companies">Sheet1!$A$1:$D$8</definedName>
     <definedName name="MoreCompanies">MoreCompanies!$A$1:$D$4</definedName>
     <definedName name="NullCellCompanies">NullCells!$A$1:$D$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">AutoFiltered!$A$1:$B$6</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">AutoFiltered!$A$1:$B$6</definedName>
     <definedName name="Range1">'Paul''s Worksheet'!$A$1:$D$11</definedName>
     <definedName name="Range2">'Paul''s Worksheet'!$A$1:$D$11</definedName>
-    <definedName name="Range3" localSheetId="5">'Paul''s Worksheet'!$E$5:$H$16</definedName>
+    <definedName name="Range3" localSheetId="6">'Paul''s Worksheet'!$E$5:$H$16</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +143,18 @@
   </si>
   <si>
     <t>Who Cares</t>
+  </si>
+  <si>
+    <t>InitiationDate</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -181,6 +199,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -229,7 +250,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,7 +285,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -479,14 +500,14 @@
       <selection activeCell="D8" sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -514,7 +535,7 @@
         <v>6890</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -528,7 +549,7 @@
         <v>34554</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -542,7 +563,7 @@
         <v>6454</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -556,7 +577,7 @@
         <v>19162</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -570,7 +591,7 @@
         <v>22182</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -584,7 +605,7 @@
         <v>39730</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -609,232 +630,230 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
+      <c r="B2">
         <v>25</v>
       </c>
-      <c r="D2" s="1">
+      <c r="C2" s="1">
         <v>6890</v>
       </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
       <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="G2">
+      <c r="F2">
         <v>255</v>
       </c>
-      <c r="H2" s="1">
+      <c r="G2" s="1">
         <v>12268</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+      <c r="B3">
         <v>98</v>
       </c>
-      <c r="D3" s="1">
+      <c r="C3" s="1">
         <v>34554</v>
       </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
       <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
         <v>25</v>
       </c>
-      <c r="G3">
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="H3" s="1">
+      <c r="G3" s="1">
         <v>36412</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
+      <c r="B4">
         <v>300</v>
       </c>
-      <c r="D4" s="1">
+      <c r="C4" s="1">
         <v>6454</v>
       </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
       <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="G4">
+      <c r="F4">
         <v>400</v>
       </c>
-      <c r="H4" s="1">
+      <c r="G4" s="1">
         <v>32350</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
+      <c r="B5">
         <v>29839</v>
       </c>
-      <c r="D5" s="1">
+      <c r="C5" s="1">
         <v>19162</v>
       </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
       <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="G5">
+      <c r="F5">
         <v>9</v>
       </c>
-      <c r="H5" s="1">
+      <c r="G5" s="1">
         <v>28359</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="D6" s="1">
+      <c r="C6" s="1">
         <v>22182</v>
       </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
       <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="G6">
+      <c r="F6">
         <v>612</v>
       </c>
-      <c r="H6" s="1">
+      <c r="G6" s="1">
         <v>16710</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="C7" s="1">
         <v>39730</v>
       </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
       <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="G7">
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="H7" s="1">
+      <c r="G7" s="1">
         <v>38868</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
+      <c r="B8">
         <v>433</v>
       </c>
-      <c r="D8" s="1">
+      <c r="C8" s="1">
         <v>29456</v>
       </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
       <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
         <v>35</v>
       </c>
-      <c r="G8">
+      <c r="F8">
         <v>3820</v>
       </c>
-      <c r="H8" s="1">
+      <c r="G8" s="1">
         <v>26394</v>
       </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -842,20 +861,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:D4"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -868,8 +892,20 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -882,8 +918,20 @@
       <c r="D2" s="1">
         <v>6890</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>255</v>
+      </c>
+      <c r="H2" s="1">
+        <v>12268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -896,8 +944,20 @@
       <c r="D3" s="1">
         <v>34554</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1">
+        <v>36412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -909,6 +969,122 @@
       </c>
       <c r="D4" s="1">
         <v>6454</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4">
+        <v>400</v>
+      </c>
+      <c r="H4" s="1">
+        <v>32350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>29839</v>
+      </c>
+      <c r="D5" s="1">
+        <v>19162</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1">
+        <v>28359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>22182</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6">
+        <v>612</v>
+      </c>
+      <c r="H6" s="1">
+        <v>16710</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>39730</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>38868</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>433</v>
+      </c>
+      <c r="D8" s="1">
+        <v>29456</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8">
+        <v>3820</v>
+      </c>
+      <c r="H8" s="1">
+        <v>26394</v>
       </c>
     </row>
   </sheetData>
@@ -920,20 +1096,98 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="A1:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6890</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>98</v>
+      </c>
+      <c r="D3" s="1">
+        <v>34554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>300</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6454</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -947,7 +1201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -961,7 +1215,7 @@
         <v>6890</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -975,7 +1229,7 @@
         <v>34554</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -989,7 +1243,7 @@
         <v>6454</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1003,7 +1257,7 @@
         <v>19162</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1017,7 +1271,7 @@
         <v>22182</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1031,7 +1285,7 @@
         <v>39730</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1053,22 +1307,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1096,7 +1350,7 @@
         <v>6890</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1107,7 +1361,7 @@
         <v>34554</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1124,7 +1378,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1132,7 +1386,7 @@
       <selection activeCell="E5" sqref="E5:H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>